<commit_message>
Update documents to latest
</commit_message>
<xml_diff>
--- a/Ensek_Agile_Delivery_Test_Analysis.xlsx
+++ b/Ensek_Agile_Delivery_Test_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\Paul\Documents\Ensek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09230D19-397D-4232-ADA9-BE7C6486E848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA58A46-1D23-424C-A6B4-07280D77F060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30255" yWindow="870" windowWidth="23820" windowHeight="15510" xr2:uid="{26EA9FD1-A948-442A-AD3A-68A3B04DCA13}"/>
+    <workbookView xWindow="25110" yWindow="1410" windowWidth="23820" windowHeight="15510" activeTab="1" xr2:uid="{26EA9FD1-A948-442A-AD3A-68A3B04DCA13}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -95,9 +95,6 @@
     <t xml:space="preserve">Olga </t>
   </si>
   <si>
-    <t xml:space="preserve">Oli </t>
-  </si>
-  <si>
     <t>Ops Team</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Sales</t>
   </si>
   <si>
-    <t xml:space="preserve">Prish </t>
-  </si>
-  <si>
     <t>Project Manager</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
   </si>
   <si>
     <t>Retro</t>
-  </si>
-  <si>
-    <t>Didn't attend stand-ups, and wasn't aware of scope changing</t>
   </si>
   <si>
     <t>Review</t>
@@ -167,56 +158,77 @@
     <t>Items rolled from the last sprint. Some PBIs were completed. but 1 PBI was not completed, and one unstarted PBI rolled to the next sprint. Sprint scope was compromised by adding a PBI that was not ready.</t>
   </si>
   <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>Product Backlog</t>
+  </si>
+  <si>
+    <t>Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Didn't appear to create one as an output of the sprint</t>
+  </si>
+  <si>
+    <t>Late for stand ups. Needs to engage the developers with refinements so that they know whats coming up, and that items are ready. Seems to interrupt the developers a lot while they are working. Didn't add details to the new PBIs quickly, but need to raise any blockers.</t>
+  </si>
+  <si>
+    <t>Was asked by Patty for details of a PBI</t>
+  </si>
+  <si>
+    <t>Cathy</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Asked PO for status, asked team to work late</t>
+  </si>
+  <si>
+    <t>Asked to work late by Cathy</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Agreed to drop current work and context switch. Complered 3 items on the sprint in isolation, and started, but didn't finish another item</t>
+  </si>
+  <si>
+    <t>Wasn't mentioned much, what did she do?</t>
+  </si>
+  <si>
+    <t>Took on Debs' work for Prish</t>
+  </si>
+  <si>
+    <t>Asked to work late by Cathy. Worked on Prish's item but context switched.</t>
+  </si>
+  <si>
     <t>Works late to test PBI 58712.
-Struggled with the test environment</t>
-  </si>
-  <si>
-    <t>Artifact</t>
-  </si>
-  <si>
-    <t>Increment</t>
-  </si>
-  <si>
-    <t>Product Backlog</t>
-  </si>
-  <si>
-    <t>Sprint Backlog</t>
-  </si>
-  <si>
-    <t>Didn't appear to create one as an output of the sprint</t>
-  </si>
-  <si>
-    <t>Skipped one standup</t>
-  </si>
-  <si>
-    <t>Late for stand ups. Needs to engage the developers with refinements so that they know whats coming up, and that items are ready. Seems to interrupt the developers a lot while they are working. Didn't add details to the new PBIs quickly, but need to raise any blockers.</t>
-  </si>
-  <si>
-    <t>Was asked by Patty for details of a PBI</t>
-  </si>
-  <si>
-    <t>Patty late. Some people have sporadic attendance. Cancelled once. Its OK to have lots of people at the stand up, but only the scrum team can participate, unless the team want to actively ask questions. Others should observe. Scum team members should set daily targets and discuss how they are progressing towards the sprint goal, and what to do next.</t>
-  </si>
-  <si>
-    <t>Cathy</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Asked PO for status, asked team to work late</t>
-  </si>
-  <si>
-    <t>Asked to work late by Cathy</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Agreed to drop current work and context switch. Complered 3 items on the sprint in isolation, and started, but didn't finish another item</t>
-  </si>
-  <si>
-    <t>Wasn't mentioned much, what did she do?</t>
+Struggled with the test environment. Had a holiday</t>
+  </si>
+  <si>
+    <t>Skipped one standup. Ran manual regression</t>
+  </si>
+  <si>
+    <t>Oli</t>
+  </si>
+  <si>
+    <t>Not involved</t>
+  </si>
+  <si>
+    <t>Sometime didn't turn up to the stand-up, sometimes interrupted. Escalated issue to Cathy</t>
+  </si>
+  <si>
+    <t>Prish</t>
+  </si>
+  <si>
+    <t>Didn't attend stand-ups, and wasn't aware of scope changing. Interrupts the stand up. Talks to the team rather than through the PO</t>
+  </si>
+  <si>
+    <t>Patty late. Some people have sporadic attendance. Cancelled once. Its OK to have lots of people at the stand up, but only the scrum team can participate, unless the team want to actively ask questions. Others should observe. Scrum team members should set daily targets and discuss how they are progressing towards the sprint goal, and what to do next.</t>
   </si>
 </sst>
 </file>
@@ -776,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6FD5B1-08D7-4F97-AA32-560A2437F32E}">
   <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +815,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -822,18 +834,20 @@
         <v>4</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -844,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -856,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -868,10 +882,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -880,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -892,7 +906,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -904,24 +918,24 @@
         <v>17</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
@@ -930,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -939,49 +953,55 @@
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="15"/>
+        <v>19</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18" s="17"/>
     </row>
@@ -999,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF22698-3C1D-4610-A19C-4E8A3400B2AA}">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1032,7 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>2</v>
@@ -1020,47 +1040,47 @@
     </row>
     <row r="3" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="135" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="17"/>
     </row>
@@ -1074,7 +1094,7 @@
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1106,7 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>2</v>
@@ -1094,21 +1114,21 @@
     </row>
     <row r="3" spans="2:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="8"/>
     </row>

</xml_diff>